<commit_message>
modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/Correction for TRTS-4S.ipynb" 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/TRTS-4S\345\261\217\346\237\265\347\267\232.xlsx" 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/\346\240\241\344\274\260.xlsx"
</commit_message>
<xml_diff>
--- a/ta/指派結果/TRTS-4S屏柵線.xlsx
+++ b/ta/指派結果/TRTS-4S屏柵線.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\暫存\Traffic-Assignment-Model\ta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\暫存\Traffic-Assignment-Model\ta\指派結果\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E615AD8-F6CB-42A9-BBD0-55FC17003F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A3B03A-8FFC-4B9B-B80D-13DE1034D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E705DE73-7DBA-4EF4-BE7B-111AF8D99A31}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{E705DE73-7DBA-4EF4-BE7B-111AF8D99A31}"/>
   </bookViews>
   <sheets>
     <sheet name="節點編號" sheetId="1" r:id="rId1"/>
@@ -1446,7 +1446,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1561,13 +1561,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1591,12 +1588,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1606,11 +1597,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1950,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B91B70-CCE3-4F38-82D1-372C96A2E9C6}">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2149,8 +2143,8 @@
       <c r="H9">
         <v>6312</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
@@ -3215,8 +3209,8 @@
       <c r="H62">
         <v>5341</v>
       </c>
-      <c r="J62" s="53"/>
-      <c r="K62" s="54"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="31"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
@@ -3349,16 +3343,16 @@
         <v>213</v>
       </c>
       <c r="D69">
-        <v>6168</v>
+        <v>5931</v>
       </c>
       <c r="E69">
-        <v>6137</v>
+        <v>5932</v>
       </c>
       <c r="G69">
-        <v>6137</v>
+        <v>7670</v>
       </c>
       <c r="H69">
-        <v>6168</v>
+        <v>5923</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3581,7 +3575,7 @@
         <v>6096</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:17">
       <c r="A81" s="1" t="s">
         <v>39</v>
       </c>
@@ -3601,7 +3595,7 @@
         <v>6010</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:17">
       <c r="A82" s="1" t="s">
         <v>39</v>
       </c>
@@ -3624,7 +3618,7 @@
         <v>6006</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:17">
       <c r="A83" s="1" t="s">
         <v>39</v>
       </c>
@@ -3643,64 +3637,62 @@
       <c r="H83">
         <v>6180</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="J83" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="M83">
+        <v>6001</v>
+      </c>
+      <c r="N83">
+        <v>7699</v>
+      </c>
+      <c r="P83">
+        <v>7699</v>
+      </c>
+      <c r="Q83">
+        <v>6001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>308</v>
+        <v>235</v>
       </c>
       <c r="D84">
-        <v>6001</v>
+        <v>6175</v>
       </c>
       <c r="E84">
-        <v>7699</v>
+        <v>6174</v>
       </c>
       <c r="G84">
-        <v>7699</v>
+        <v>6174</v>
       </c>
       <c r="H84">
-        <v>6001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>6175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
       <c r="A85" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D85">
-        <v>6175</v>
+        <v>6146</v>
       </c>
       <c r="E85">
-        <v>6174</v>
+        <v>16133</v>
       </c>
       <c r="G85">
-        <v>6174</v>
+        <v>16133</v>
       </c>
       <c r="H85">
-        <v>6175</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D86">
-        <v>6146</v>
-      </c>
-      <c r="E86">
-        <v>16133</v>
-      </c>
-      <c r="G86">
-        <v>16133</v>
-      </c>
-      <c r="H86">
         <v>6146</v>
       </c>
     </row>
@@ -4688,6 +4680,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -4700,11 +4697,6 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4717,7 +4709,7 @@
   <dimension ref="A1:O226"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:L59"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4745,18 +4737,18 @@
     <row r="1" spans="1:15">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
       <c r="N1" s="14" t="s">
         <v>87</v>
       </c>
@@ -4765,26 +4757,26 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="50" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="49"/>
       <c r="N2" s="1" t="s">
         <v>90</v>
       </c>
@@ -4793,8 +4785,8 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="42"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="3" t="s">
         <v>51</v>
       </c>
@@ -5959,7 +5951,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="38"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="21" t="s">
         <v>63</v>
       </c>
@@ -6013,18 +6005,18 @@
     <row r="31" spans="1:15">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
       <c r="N31" s="1" t="s">
         <v>137</v>
       </c>
@@ -6033,26 +6025,26 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="45" t="s">
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="47"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="46"/>
       <c r="N32" s="1" t="s">
         <v>139</v>
       </c>
@@ -6061,8 +6053,8 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="42"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -7227,7 +7219,7 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="38"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="21" t="s">
         <v>63</v>
       </c>
@@ -8047,6 +8039,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -8059,30 +8075,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   ta/Taipei/no_left_turns.dat 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/Correction for TRTS-4S.ipynb" 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/TRTS-4S\345\261\217\346\237\265\347\267\232.xlsx"
</commit_message>
<xml_diff>
--- a/ta/指派結果/TRTS-4S屏柵線.xlsx
+++ b/ta/指派結果/TRTS-4S屏柵線.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\暫存\Traffic-Assignment-Model\ta\指派結果\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5380849E-9B16-4C0F-B836-D2DAD92260DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC09388D-BAF2-46BB-B501-20BCC5490DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{E705DE73-7DBA-4EF4-BE7B-111AF8D99A31}"/>
+    <workbookView xWindow="3825" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{E705DE73-7DBA-4EF4-BE7B-111AF8D99A31}"/>
   </bookViews>
   <sheets>
     <sheet name="節點編號" sheetId="1" r:id="rId1"/>
@@ -1104,14 +1104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>建國北路(國一往北)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建國北路(國一往南)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中山北路(慢車道)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1129,6 +1121,14 @@
   </si>
   <si>
     <t>SL2</t>
+  </si>
+  <si>
+    <t>建國北路高架(國一往北)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建國北路平面(國一往南)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1446,7 +1446,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1561,10 +1561,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1588,6 +1591,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1596,21 +1605,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1952,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B91B70-CCE3-4F38-82D1-372C96A2E9C6}">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2167,8 +2161,8 @@
       <c r="H9">
         <v>6312</v>
       </c>
-      <c r="J9" s="53"/>
-      <c r="K9" s="54"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
@@ -2392,7 +2386,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>107</v>
@@ -2412,7 +2406,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>109</v>
@@ -2432,7 +2426,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>111</v>
@@ -2452,7 +2446,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>113</v>
@@ -2472,10 +2466,10 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D25">
         <v>8371</v>
@@ -2492,7 +2486,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>115</v>
@@ -2512,7 +2506,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>117</v>
@@ -2532,7 +2526,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>119</v>
@@ -2552,7 +2546,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>121</v>
@@ -2572,10 +2566,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D30">
         <v>8432</v>
@@ -2592,7 +2586,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>123</v>
@@ -2612,7 +2606,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>125</v>
@@ -2632,10 +2626,10 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D33">
         <v>8535</v>
@@ -2652,7 +2646,7 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>127</v>
@@ -2672,7 +2666,7 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>131</v>
@@ -2692,7 +2686,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>133</v>
@@ -2712,10 +2706,10 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D37">
         <v>7771</v>
@@ -2732,7 +2726,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>135</v>
@@ -2752,7 +2746,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>138</v>
@@ -2774,7 +2768,7 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>140</v>
@@ -2794,7 +2788,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>142</v>
@@ -2814,7 +2808,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>144</v>
@@ -2834,7 +2828,7 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>146</v>
@@ -2854,7 +2848,7 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>148</v>
@@ -2874,7 +2868,7 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>150</v>
@@ -2897,13 +2891,13 @@
         <v>309</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D46">
-        <v>6645</v>
+        <v>6382</v>
       </c>
       <c r="E46">
-        <v>6691</v>
+        <v>6383</v>
       </c>
       <c r="G46">
         <v>6381</v>
@@ -2917,13 +2911,13 @@
         <v>309</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D47">
-        <v>6324</v>
+        <v>6690</v>
       </c>
       <c r="E47">
-        <v>6382</v>
+        <v>6359</v>
       </c>
       <c r="G47">
         <v>6384</v>
@@ -3233,8 +3227,8 @@
       <c r="H62">
         <v>5341</v>
       </c>
-      <c r="J62" s="53"/>
-      <c r="K62" s="54"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="31"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
@@ -4704,11 +4698,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -4721,6 +4710,11 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4761,18 +4755,18 @@
     <row r="1" spans="1:15">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
       <c r="N1" s="14" t="s">
         <v>87</v>
       </c>
@@ -4781,26 +4775,26 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47" t="s">
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="49"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="52"/>
       <c r="N2" s="1" t="s">
         <v>90</v>
       </c>
@@ -4809,8 +4803,8 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="41"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="3" t="s">
         <v>51</v>
       </c>
@@ -5975,7 +5969,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="50"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="21" t="s">
         <v>63</v>
       </c>
@@ -6029,18 +6023,18 @@
     <row r="31" spans="1:15">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
       <c r="N31" s="1" t="s">
         <v>137</v>
       </c>
@@ -6049,26 +6043,26 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="44" t="s">
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="47"/>
       <c r="N32" s="1" t="s">
         <v>139</v>
       </c>
@@ -6077,8 +6071,8 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="41"/>
-      <c r="B33" s="43"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -7243,7 +7237,7 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="50"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="21" t="s">
         <v>63</v>
       </c>
@@ -8063,6 +8057,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:L32"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
@@ -8075,30 +8093,6 @@
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A56:A57"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAPE計算: 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/Correction for TRTS-4S.ipynb" 	modified:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/TRTS-4S\345\261\217\346\237\265\347\267\232.xlsx" 	new file:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/\346\230\217\345\263\260\346\240\241\344\274\260.txt" 	new file:   "ta/\346\214\207\346\264\276\347\265\220\346\236\234/\346\231\250\345\263\260\346\240\241\344\274\260.txt"
</commit_message>
<xml_diff>
--- a/ta/指派結果/TRTS-4S屏柵線.xlsx
+++ b/ta/指派結果/TRTS-4S屏柵線.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\暫存\Traffic-Assignment-Model\ta\指派結果\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BDE360-85B6-4C7C-856B-19F7543B4818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63CBBF3-6833-4917-B4C4-106527408DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{E705DE73-7DBA-4EF4-BE7B-111AF8D99A31}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="363">
   <si>
     <t>group</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1219,6 +1219,10 @@
   </si>
   <si>
     <t>國一平面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SL11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1789,13 +1793,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1819,12 +1820,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1833,6 +1828,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2174,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B91B70-CCE3-4F38-82D1-372C96A2E9C6}">
   <dimension ref="A1:Q140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="K128" sqref="K128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5601,7 +5605,7 @@
     </row>
     <row r="130" spans="1:8">
       <c r="A130" s="31" t="s">
-        <v>80</v>
+        <v>362</v>
       </c>
       <c r="B130" s="31" t="s">
         <v>277</v>
@@ -6553,6 +6557,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -6565,11 +6574,6 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6927,18 +6931,18 @@
     <row r="1" spans="1:15">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
       <c r="N1" s="14" t="s">
         <v>85</v>
       </c>
@@ -6947,26 +6951,26 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="64" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="66"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
       <c r="N2" s="1" t="s">
         <v>88</v>
       </c>
@@ -6975,8 +6979,8 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="3" t="s">
         <v>49</v>
       </c>
@@ -8141,7 +8145,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="52"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="21" t="s">
         <v>61</v>
       </c>
@@ -8195,18 +8199,18 @@
     <row r="31" spans="1:15">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="53" t="s">
+      <c r="C31" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
       <c r="N31" s="1" t="s">
         <v>135</v>
       </c>
@@ -8215,26 +8219,26 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="59" t="s">
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="61"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="60"/>
       <c r="N32" s="1" t="s">
         <v>137</v>
       </c>
@@ -8243,8 +8247,8 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="56"/>
-      <c r="B33" s="58"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="57"/>
       <c r="C33" s="3" t="s">
         <v>49</v>
       </c>
@@ -9409,7 +9413,7 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="52"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="21" t="s">
         <v>61</v>
       </c>
@@ -10229,6 +10233,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -10241,30 +10269,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>